<commit_message>
ClickDetectorSpeller codebase should be complete.
</commit_message>
<xml_diff>
--- a/Analysis/MainFigures/SourceData/switch_scanning_spelling_metrics.xlsx
+++ b/Analysis/MainFigures/SourceData/switch_scanning_spelling_metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DANCAN~1\DOCUME~1\MobaXterm\slash\RemoteFiles\1773934_2_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanCandrea\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8E8D30-5BF8-4E70-A231-8153E39A7394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE535695-9E6C-48FD-BBEE-58EBDCEB7929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39705" yWindow="2505" windowWidth="32100" windowHeight="15780" activeTab="1" xr2:uid="{79707531-4519-46E9-8260-C7BB790F6B62}"/>
+    <workbookView xWindow="4485" yWindow="3015" windowWidth="32100" windowHeight="15780" activeTab="1" xr2:uid="{79707531-4519-46E9-8260-C7BB790F6B62}"/>
   </bookViews>
   <sheets>
     <sheet name="4_votes" sheetId="2" r:id="rId1"/>
@@ -95,12 +95,6 @@
   </si>
   <si>
     <t>2023_01_12</t>
-  </si>
-  <si>
-    <t>Mean Latency to NAVI (s)</t>
-  </si>
-  <si>
-    <t>Stdev Latency to NAVI (s)</t>
   </si>
   <si>
     <t>2022_12_15_Total</t>
@@ -206,6 +200,12 @@
   </si>
   <si>
     <t>Wrong CPM</t>
+  </si>
+  <si>
+    <t>Mean Latency to UI (s)</t>
+  </si>
+  <si>
+    <t>Stdev Latency to UI (s)</t>
   </si>
 </sst>
 </file>
@@ -546,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -821,9 +821,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1281,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD4F3BB8-9995-4F95-B690-EFC1C4CF5960}">
   <dimension ref="A1:AE52"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1311,19 +1308,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>9</v>
@@ -1332,16 +1329,16 @@
         <v>15</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>7</v>
@@ -1350,10 +1347,10 @@
         <v>8</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>13</v>
@@ -1365,13 +1362,13 @@
         <v>12</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -1417,7 +1414,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="7">
-        <v>0.501</v>
+        <v>0.502</v>
       </c>
       <c r="N2" s="7">
         <v>8.1000000000000003E-2</v>
@@ -1442,10 +1439,10 @@
         <f t="shared" ref="T2:T36" si="6">S2/(G2/60)</f>
         <v>2.6213228038512351</v>
       </c>
-      <c r="U2" s="145">
-        <v>0</v>
-      </c>
-      <c r="V2" s="145">
+      <c r="U2" s="144">
+        <v>0</v>
+      </c>
+      <c r="V2" s="144">
         <f xml:space="preserve"> U2/(G2/60)</f>
         <v>0</v>
       </c>
@@ -1455,13 +1452,13 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="19">
         <v>81</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="71">
         <f>SUM(D2)</f>
@@ -1499,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="6">
-        <v>0.501</v>
+        <v>0.502</v>
       </c>
       <c r="N3" s="6">
         <v>8.1000000000000003E-2</v>
@@ -1524,11 +1521,11 @@
         <f t="shared" si="6"/>
         <v>2.6213228038512351</v>
       </c>
-      <c r="U3" s="146">
+      <c r="U3" s="145">
         <f>SUM(U2)</f>
         <v>0</v>
       </c>
-      <c r="V3" s="147">
+      <c r="V3" s="146">
         <f t="shared" ref="V3:V36" si="7" xml:space="preserve"> U3/(G3/60)</f>
         <v>0</v>
       </c>
@@ -1582,7 +1579,7 @@
         <v>0.41799999999999998</v>
       </c>
       <c r="N4" s="18">
-        <v>0.113</v>
+        <v>0.112</v>
       </c>
       <c r="O4" s="18">
         <v>0.61199999999999999</v>
@@ -1604,10 +1601,10 @@
         <f t="shared" si="6"/>
         <v>2.6245230901329273</v>
       </c>
-      <c r="U4" s="145">
-        <v>0</v>
-      </c>
-      <c r="V4" s="145">
+      <c r="U4" s="144">
+        <v>0</v>
+      </c>
+      <c r="V4" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -1661,7 +1658,7 @@
         <v>0.42799999999999999</v>
       </c>
       <c r="N5" s="7">
-        <v>0.09</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="O5" s="7">
         <v>0.63</v>
@@ -1683,10 +1680,10 @@
         <f t="shared" si="6"/>
         <v>2.4356365394899635</v>
       </c>
-      <c r="U5" s="145">
-        <v>0</v>
-      </c>
-      <c r="V5" s="145">
+      <c r="U5" s="144">
+        <v>0</v>
+      </c>
+      <c r="V5" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -1737,7 +1734,7 @@
         <v>0.53858444619413148</v>
       </c>
       <c r="M6" s="7">
-        <v>0.47099999999999997</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="N6" s="7">
         <v>0.10199999999999999</v>
@@ -1762,10 +1759,10 @@
         <f t="shared" si="6"/>
         <v>1.8465752440941652</v>
       </c>
-      <c r="U6" s="145">
+      <c r="U6" s="144">
         <v>7</v>
       </c>
-      <c r="V6" s="145">
+      <c r="V6" s="144">
         <f t="shared" si="7"/>
         <v>0.53858444619413148</v>
       </c>
@@ -1816,16 +1813,16 @@
         <v>0.60822581976531176</v>
       </c>
       <c r="M7" s="7">
-        <v>0.48</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="N7" s="7">
         <v>0.114</v>
       </c>
       <c r="O7" s="7">
-        <v>0.66100000000000003</v>
+        <v>0.65900000000000003</v>
       </c>
       <c r="P7" s="7">
-        <v>0.128</v>
+        <v>0.129</v>
       </c>
       <c r="Q7" s="7">
         <v>114</v>
@@ -1841,10 +1838,10 @@
         <f t="shared" si="6"/>
         <v>2.085345667766783</v>
       </c>
-      <c r="U7" s="145">
+      <c r="U7" s="144">
         <v>1</v>
       </c>
-      <c r="V7" s="145">
+      <c r="V7" s="144">
         <f t="shared" si="7"/>
         <v>8.6889402823615958E-2</v>
       </c>
@@ -1854,13 +1851,13 @@
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="19">
         <v>83</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="23">
         <f>SUM(D4:D7)</f>
@@ -1899,13 +1896,13 @@
         <v>0.40690272801905808</v>
       </c>
       <c r="M8" s="23">
-        <v>0.46</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="N8" s="23">
-        <v>0.11600000000000001</v>
+        <v>0.109</v>
       </c>
       <c r="O8" s="23">
-        <v>0.64400000000000002</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="P8" s="23">
         <v>0.12</v>
@@ -1926,11 +1923,11 @@
         <f>S8/(G8/60)</f>
         <v>2.2153592969926494</v>
       </c>
-      <c r="U8" s="146">
+      <c r="U8" s="145">
         <f>SUM(U4:U7)</f>
         <v>8</v>
       </c>
-      <c r="V8" s="147">
+      <c r="V8" s="146">
         <f t="shared" si="7"/>
         <v>0.18084565689735915</v>
       </c>
@@ -1981,7 +1978,7 @@
         <v>0.18442301722203608</v>
       </c>
       <c r="M9" s="18">
-        <v>0.45200000000000001</v>
+        <v>0.48499999999999999</v>
       </c>
       <c r="N9" s="18">
         <v>0.09</v>
@@ -2006,10 +2003,10 @@
         <f t="shared" si="6"/>
         <v>2.1208646980534152</v>
       </c>
-      <c r="U9" s="145">
+      <c r="U9" s="144">
         <v>1</v>
       </c>
-      <c r="V9" s="145">
+      <c r="V9" s="144">
         <f t="shared" si="7"/>
         <v>9.2211508611018053E-2</v>
       </c>
@@ -2060,10 +2057,10 @@
         <v>0.31587592393707747</v>
       </c>
       <c r="M10" s="7">
-        <v>0.46300000000000002</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="N10" s="7">
-        <v>9.4E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="O10" s="7">
         <v>0.66800000000000004</v>
@@ -2085,10 +2082,10 @@
         <f t="shared" si="6"/>
         <v>2.1058394929138498</v>
       </c>
-      <c r="U10" s="145">
+      <c r="U10" s="144">
         <v>2</v>
       </c>
-      <c r="V10" s="145">
+      <c r="V10" s="144">
         <f t="shared" si="7"/>
         <v>0.21058394929138499</v>
       </c>
@@ -2139,7 +2136,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="7">
-        <v>0.51600000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="N11" s="7">
         <v>9.2999999999999999E-2</v>
@@ -2164,10 +2161,10 @@
         <f t="shared" si="6"/>
         <v>1.8425056848977486</v>
       </c>
-      <c r="U11" s="145">
+      <c r="U11" s="144">
         <v>2</v>
       </c>
-      <c r="V11" s="145">
+      <c r="V11" s="144">
         <f t="shared" si="7"/>
         <v>0.18425056848977486</v>
       </c>
@@ -2218,10 +2215,10 @@
         <v>0</v>
       </c>
       <c r="M12" s="7">
-        <v>0.5</v>
+        <v>0.502</v>
       </c>
       <c r="N12" s="7">
-        <v>7.9000000000000001E-2</v>
+        <v>0.08</v>
       </c>
       <c r="O12" s="7">
         <v>0.69499999999999995</v>
@@ -2243,10 +2240,10 @@
         <f t="shared" si="6"/>
         <v>2.1845422397929539</v>
       </c>
-      <c r="U12" s="145">
-        <v>0</v>
-      </c>
-      <c r="V12" s="145">
+      <c r="U12" s="144">
+        <v>0</v>
+      </c>
+      <c r="V12" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2297,10 +2294,10 @@
         <v>0</v>
       </c>
       <c r="M13" s="7">
-        <v>0.499</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="N13" s="7">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="O13" s="7">
         <v>0.71899999999999997</v>
@@ -2322,10 +2319,10 @@
         <f t="shared" si="6"/>
         <v>2.4493378283218297</v>
       </c>
-      <c r="U13" s="145">
-        <v>0</v>
-      </c>
-      <c r="V13" s="145">
+      <c r="U13" s="144">
+        <v>0</v>
+      </c>
+      <c r="V13" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2335,13 +2332,13 @@
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="19">
         <v>84</v>
       </c>
       <c r="C14" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14" s="23">
         <f>SUM(D9:D13)</f>
@@ -2380,10 +2377,10 @@
         <v>9.6187758504600984E-2</v>
       </c>
       <c r="M14" s="6">
-        <v>0.48599999999999999</v>
+        <v>0.49299999999999999</v>
       </c>
       <c r="N14" s="6">
-        <v>9.1999999999999998E-2</v>
+        <v>0.09</v>
       </c>
       <c r="O14" s="6">
         <v>0.69199999999999995</v>
@@ -2407,11 +2404,11 @@
         <f t="shared" si="6"/>
         <v>2.1353682388021418</v>
       </c>
-      <c r="U14" s="146">
+      <c r="U14" s="145">
         <f>SUM(U9:U13)</f>
         <v>5</v>
       </c>
-      <c r="V14" s="147">
+      <c r="V14" s="146">
         <f t="shared" si="7"/>
         <v>9.6187758504600984E-2</v>
       </c>
@@ -2462,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="18">
-        <v>0.503</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="N15" s="18">
         <v>6.4000000000000001E-2</v>
@@ -2487,10 +2484,10 @@
         <f t="shared" si="6"/>
         <v>2.5436466643542603</v>
       </c>
-      <c r="U15" s="145">
+      <c r="U15" s="144">
         <v>1</v>
       </c>
-      <c r="V15" s="145">
+      <c r="V15" s="144">
         <f t="shared" si="7"/>
         <v>0.11562030292519365</v>
       </c>
@@ -2541,7 +2538,7 @@
         <v>0.11076609523668868</v>
       </c>
       <c r="M16" s="7">
-        <v>0.48199999999999998</v>
+        <v>0.48299999999999998</v>
       </c>
       <c r="N16" s="7">
         <v>8.7999999999999995E-2</v>
@@ -2566,10 +2563,10 @@
         <f t="shared" si="6"/>
         <v>2.3260879999704622</v>
       </c>
-      <c r="U16" s="145">
+      <c r="U16" s="144">
         <v>1</v>
       </c>
-      <c r="V16" s="145">
+      <c r="V16" s="144">
         <f t="shared" si="7"/>
         <v>0.11076609523668869</v>
       </c>
@@ -2579,13 +2576,13 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="19">
         <v>87</v>
       </c>
       <c r="C17" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D17" s="23">
         <f>SUM(D15:D16)</f>
@@ -2624,10 +2621,10 @@
         <v>5.6570578396450383E-2</v>
       </c>
       <c r="M17" s="6">
-        <v>0.49199999999999999</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="N17" s="6">
-        <v>7.8E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="O17" s="6">
         <v>0.70199999999999996</v>
@@ -2651,11 +2648,11 @@
         <f t="shared" si="6"/>
         <v>2.4325348710473667</v>
       </c>
-      <c r="U17" s="146">
+      <c r="U17" s="145">
         <f>SUM(U15:U16)</f>
         <v>2</v>
       </c>
-      <c r="V17" s="147">
+      <c r="V17" s="146">
         <f t="shared" si="7"/>
         <v>0.11314115679290077</v>
       </c>
@@ -2706,10 +2703,10 @@
         <v>0.72776672650526419</v>
       </c>
       <c r="M18" s="18">
-        <v>0.5</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="N18" s="18">
-        <v>0.115</v>
+        <v>0.113</v>
       </c>
       <c r="O18" s="18">
         <v>0.628</v>
@@ -2731,10 +2728,10 @@
         <f t="shared" si="6"/>
         <v>1.654015287511964</v>
       </c>
-      <c r="U18" s="145">
+      <c r="U18" s="144">
         <v>7</v>
       </c>
-      <c r="V18" s="145">
+      <c r="V18" s="144">
         <f t="shared" si="7"/>
         <v>0.46312428050334992</v>
       </c>
@@ -2785,10 +2782,10 @@
         <v>0.10190650078552928</v>
       </c>
       <c r="M19" s="7">
-        <v>0.45900000000000002</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="N19" s="7">
-        <v>9.6000000000000002E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="O19" s="7">
         <v>0.66100000000000003</v>
@@ -2810,10 +2807,10 @@
         <f t="shared" si="6"/>
         <v>2.4457560188527028</v>
       </c>
-      <c r="U19" s="145">
+      <c r="U19" s="144">
         <v>1</v>
       </c>
-      <c r="V19" s="145">
+      <c r="V19" s="144">
         <f t="shared" si="7"/>
         <v>0.10190650078552928</v>
       </c>
@@ -2823,13 +2820,13 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" s="19">
         <v>89</v>
       </c>
       <c r="C20" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" s="23">
         <f>SUM(D18:D19)</f>
@@ -2868,16 +2865,16 @@
         <v>0.48139315178125491</v>
       </c>
       <c r="M20" s="6">
-        <v>0.47299999999999998</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="N20" s="6">
-        <v>0.108</v>
+        <v>0.106</v>
       </c>
       <c r="O20" s="6">
-        <v>0.65200000000000002</v>
+        <v>0.64200000000000002</v>
       </c>
       <c r="P20" s="6">
-        <v>0.121</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="Q20" s="6">
         <f>SUM(Q18:Q19)</f>
@@ -2895,11 +2892,11 @@
         <f t="shared" si="6"/>
         <v>1.9656887031067909</v>
       </c>
-      <c r="U20" s="146">
+      <c r="U20" s="145">
         <f>SUM(U18:U19)</f>
         <v>8</v>
       </c>
-      <c r="V20" s="147">
+      <c r="V20" s="146">
         <f t="shared" si="7"/>
         <v>0.32092876785416991</v>
       </c>
@@ -2950,16 +2947,16 @@
         <v>0.21387705633878126</v>
       </c>
       <c r="M21" s="18">
-        <v>0.48199999999999998</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="N21" s="18">
-        <v>0.125</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="O21" s="18">
-        <v>0.627</v>
+        <v>0.623</v>
       </c>
       <c r="P21" s="18">
-        <v>0.126</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="Q21" s="17">
         <v>138</v>
@@ -2975,10 +2972,10 @@
         <f t="shared" si="6"/>
         <v>2.1387705633878125</v>
       </c>
-      <c r="U21" s="145">
+      <c r="U21" s="144">
         <v>5</v>
       </c>
-      <c r="V21" s="145">
+      <c r="V21" s="144">
         <f t="shared" si="7"/>
         <v>0.35646176056463541</v>
       </c>
@@ -3029,10 +3026,10 @@
         <v>0</v>
       </c>
       <c r="M22" s="7">
-        <v>0.46500000000000002</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="N22" s="7">
-        <v>0.11899999999999999</v>
+        <v>0.106</v>
       </c>
       <c r="O22" s="7">
         <v>0.63500000000000001</v>
@@ -3054,10 +3051,10 @@
         <f t="shared" si="6"/>
         <v>2.0139402426168633</v>
       </c>
-      <c r="U22" s="145">
-        <v>0</v>
-      </c>
-      <c r="V22" s="145">
+      <c r="U22" s="144">
+        <v>0</v>
+      </c>
+      <c r="V22" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3108,10 +3105,10 @@
         <v>0.4229645585911655</v>
       </c>
       <c r="M23" s="7">
-        <v>0.441</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="N23" s="7">
-        <v>0.13900000000000001</v>
+        <v>0.125</v>
       </c>
       <c r="O23" s="7">
         <v>0.61299999999999999</v>
@@ -3133,10 +3130,10 @@
         <f t="shared" si="6"/>
         <v>2.0543992845856609</v>
       </c>
-      <c r="U23" s="145">
+      <c r="U23" s="144">
         <v>7</v>
       </c>
-      <c r="V23" s="145">
+      <c r="V23" s="144">
         <f t="shared" si="7"/>
         <v>0.4229645585911655</v>
       </c>
@@ -3146,13 +3143,13 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" s="19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" s="19">
         <v>104</v>
       </c>
       <c r="C24" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D24" s="23">
         <f>SUM(D21:D23)</f>
@@ -3191,16 +3188,16 @@
         <v>0.21521181685043964</v>
       </c>
       <c r="M24" s="6">
-        <v>0.47199999999999998</v>
+        <v>0.438</v>
       </c>
       <c r="N24" s="6">
-        <v>0.122</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="O24" s="6">
-        <v>0.63100000000000001</v>
+        <v>0.624</v>
       </c>
       <c r="P24" s="6">
-        <v>0.122</v>
+        <v>0.129</v>
       </c>
       <c r="Q24" s="19">
         <f xml:space="preserve"> SUM(Q21:Q23)</f>
@@ -3218,11 +3215,11 @@
         <f t="shared" si="6"/>
         <v>2.0660334417642203</v>
       </c>
-      <c r="U24" s="146">
+      <c r="U24" s="145">
         <f>SUM(U21:U23)</f>
         <v>12</v>
       </c>
-      <c r="V24" s="147">
+      <c r="V24" s="146">
         <f t="shared" si="7"/>
         <v>0.25825418022052754</v>
       </c>
@@ -3273,7 +3270,7 @@
         <v>0.26854859554679295</v>
       </c>
       <c r="M25" s="18">
-        <v>0.51</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="N25" s="18">
         <v>8.4000000000000005E-2</v>
@@ -3298,10 +3295,10 @@
         <f t="shared" si="6"/>
         <v>1.9469773177142486</v>
       </c>
-      <c r="U25" s="145">
+      <c r="U25" s="144">
         <v>6</v>
       </c>
-      <c r="V25" s="145">
+      <c r="V25" s="144">
         <f t="shared" si="7"/>
         <v>0.40282289332018939</v>
       </c>
@@ -3352,10 +3349,10 @@
         <v>6.2285051691402485E-2</v>
       </c>
       <c r="M26" s="7">
-        <v>0.497</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="N26" s="7">
-        <v>8.2000000000000003E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="O26" s="7">
         <v>0.69</v>
@@ -3377,10 +3374,10 @@
         <f t="shared" si="6"/>
         <v>2.0554067058162819</v>
       </c>
-      <c r="U26" s="145">
+      <c r="U26" s="144">
         <v>1</v>
       </c>
-      <c r="V26" s="145">
+      <c r="V26" s="144">
         <f t="shared" si="7"/>
         <v>6.2285051691402485E-2</v>
       </c>
@@ -3431,13 +3428,13 @@
         <v>0</v>
       </c>
       <c r="M27" s="7">
-        <v>0.51800000000000002</v>
+        <v>0.52</v>
       </c>
       <c r="N27" s="7">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="O27" s="7">
-        <v>0.71399999999999997</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="P27" s="7">
         <v>9.6000000000000002E-2</v>
@@ -3456,10 +3453,10 @@
         <f t="shared" si="6"/>
         <v>2.1158213850034548</v>
       </c>
-      <c r="U27" s="145">
-        <v>0</v>
-      </c>
-      <c r="V27" s="145">
+      <c r="U27" s="144">
+        <v>0</v>
+      </c>
+      <c r="V27" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3469,13 +3466,13 @@
     </row>
     <row r="28" spans="1:25">
       <c r="A28" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28" s="19">
         <v>105</v>
       </c>
       <c r="C28" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D28" s="23">
         <f>SUM(D25:D27)</f>
@@ -3541,11 +3538,11 @@
         <f t="shared" si="6"/>
         <v>2.0401851359490388</v>
       </c>
-      <c r="U28" s="146">
+      <c r="U28" s="145">
         <f>SUM(U25:U27)</f>
         <v>7</v>
       </c>
-      <c r="V28" s="147">
+      <c r="V28" s="146">
         <f t="shared" si="7"/>
         <v>0.15192868033663054</v>
       </c>
@@ -3596,7 +3593,7 @@
         <v>6.0869644612579932E-2</v>
       </c>
       <c r="M29" s="50">
-        <v>0.45900000000000002</v>
+        <v>0.45700000000000002</v>
       </c>
       <c r="N29" s="50">
         <v>7.5999999999999998E-2</v>
@@ -3621,10 +3618,10 @@
         <f t="shared" si="6"/>
         <v>1.7043500491522383</v>
       </c>
-      <c r="U29" s="145">
+      <c r="U29" s="144">
         <v>1</v>
       </c>
-      <c r="V29" s="145">
+      <c r="V29" s="144">
         <f t="shared" si="7"/>
         <v>6.0869644612579939E-2</v>
       </c>
@@ -3675,7 +3672,7 @@
         <v>0.16910332024974681</v>
       </c>
       <c r="M30" s="1">
-        <v>0.46400000000000002</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="N30" s="1">
         <v>0.08</v>
@@ -3700,10 +3697,10 @@
         <f t="shared" si="6"/>
         <v>1.8601365227472149</v>
       </c>
-      <c r="U30" s="145">
+      <c r="U30" s="144">
         <v>2</v>
       </c>
-      <c r="V30" s="145">
+      <c r="V30" s="144">
         <f t="shared" si="7"/>
         <v>0.11273554683316453</v>
       </c>
@@ -3754,13 +3751,13 @@
         <v>6.425186731989399E-2</v>
       </c>
       <c r="M31" s="1">
-        <v>0.46100000000000002</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="N31" s="1">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="O31" s="1">
-        <v>0.67100000000000004</v>
+        <v>0.67</v>
       </c>
       <c r="P31" s="1">
         <v>9.9000000000000005E-2</v>
@@ -3779,10 +3776,10 @@
         <f t="shared" si="6"/>
         <v>2.0560597542366073</v>
       </c>
-      <c r="U31" s="145">
+      <c r="U31" s="144">
         <v>1</v>
       </c>
-      <c r="V31" s="145">
+      <c r="V31" s="144">
         <f t="shared" si="7"/>
         <v>6.4251867319893977E-2</v>
       </c>
@@ -3792,13 +3789,13 @@
     </row>
     <row r="32" spans="1:25">
       <c r="A32" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B32" s="19">
         <v>109</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D32" s="56">
         <f>SUM(D29:D31)</f>
@@ -3836,8 +3833,8 @@
         <f t="shared" si="4"/>
         <v>0.10053700163808289</v>
       </c>
-      <c r="M32" s="96">
-        <v>0.46200000000000002</v>
+      <c r="M32" s="79">
+        <v>0.45800000000000002</v>
       </c>
       <c r="N32" s="41">
         <v>0.08</v>
@@ -3864,11 +3861,11 @@
         <f t="shared" si="6"/>
         <v>1.8699882304683417</v>
       </c>
-      <c r="U32" s="146">
+      <c r="U32" s="145">
         <f>SUM(U29:U31)</f>
         <v>4</v>
       </c>
-      <c r="V32" s="147">
+      <c r="V32" s="146">
         <f t="shared" si="7"/>
         <v>8.0429601310466309E-2</v>
       </c>
@@ -3919,7 +3916,7 @@
         <v>0.14421568898444515</v>
       </c>
       <c r="M33" s="1">
-        <v>0.46200000000000002</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="N33" s="1">
         <v>7.6999999999999999E-2</v>
@@ -3944,10 +3941,10 @@
         <f t="shared" si="6"/>
         <v>2.3074510237511219</v>
       </c>
-      <c r="U33" s="145">
+      <c r="U33" s="144">
         <v>2</v>
       </c>
-      <c r="V33" s="145">
+      <c r="V33" s="144">
         <f t="shared" si="7"/>
         <v>0.14421568898444512</v>
       </c>
@@ -3998,7 +3995,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="1">
-        <v>0.47599999999999998</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="N34" s="1">
         <v>7.8E-2</v>
@@ -4023,10 +4020,10 @@
         <f t="shared" si="6"/>
         <v>2.1071115013169446</v>
       </c>
-      <c r="U34" s="145">
+      <c r="U34" s="144">
         <v>1</v>
       </c>
-      <c r="V34" s="145">
+      <c r="V34" s="144">
         <f t="shared" si="7"/>
         <v>6.1973867685792487E-2</v>
       </c>
@@ -4077,7 +4074,7 @@
         <v>6.9571912427514759E-2</v>
       </c>
       <c r="M35" s="1">
-        <v>0.49399999999999999</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="N35" s="1">
         <v>7.8E-2</v>
@@ -4102,10 +4099,10 @@
         <f t="shared" si="6"/>
         <v>2.2263011976804723</v>
       </c>
-      <c r="U35" s="145">
-        <v>0</v>
-      </c>
-      <c r="V35" s="145">
+      <c r="U35" s="144">
+        <v>0</v>
+      </c>
+      <c r="V35" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4115,13 +4112,13 @@
     </row>
     <row r="36" spans="1:31">
       <c r="A36" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B36" s="19">
         <v>111</v>
       </c>
       <c r="C36" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D36" s="56">
         <f>SUM(D33:D35)</f>
@@ -4160,10 +4157,10 @@
         <v>6.7601723693728147E-2</v>
       </c>
       <c r="M36" s="88">
-        <v>0.47699999999999998</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="N36" s="58">
-        <v>7.9000000000000001E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="O36" s="58">
         <v>0.68200000000000005</v>
@@ -4187,11 +4184,11 @@
         <f t="shared" si="6"/>
         <v>2.2083229739951191</v>
       </c>
-      <c r="U36" s="146">
+      <c r="U36" s="145">
         <f>SUM(U33:U35)</f>
         <v>3</v>
       </c>
-      <c r="V36" s="147">
+      <c r="V36" s="146">
         <f t="shared" si="7"/>
         <v>6.7601723693728133E-2</v>
       </c>
@@ -4204,7 +4201,7 @@
       <c r="B37" s="36"/>
       <c r="C37" s="36"/>
       <c r="D37" s="36"/>
-      <c r="E37" s="97"/>
+      <c r="E37" s="96"/>
       <c r="F37" s="94"/>
       <c r="G37" s="1"/>
       <c r="H37" s="48"/>
@@ -4254,26 +4251,26 @@
       <c r="Y38" s="10"/>
     </row>
     <row r="39" spans="1:31">
-      <c r="A39" s="99"/>
-      <c r="B39" s="100"/>
-      <c r="C39" s="101"/>
-      <c r="D39" s="100"/>
-      <c r="E39" s="100"/>
-      <c r="F39" s="102"/>
-      <c r="G39" s="100"/>
-      <c r="H39" s="103"/>
-      <c r="I39" s="99"/>
-      <c r="J39" s="99"/>
-      <c r="K39" s="104"/>
-      <c r="L39" s="105"/>
-      <c r="M39" s="106"/>
-      <c r="N39" s="106"/>
-      <c r="O39" s="106"/>
-      <c r="P39" s="106"/>
-      <c r="Q39" s="100"/>
-      <c r="R39" s="99"/>
-      <c r="S39" s="100"/>
-      <c r="T39" s="99"/>
+      <c r="A39" s="98"/>
+      <c r="B39" s="99"/>
+      <c r="C39" s="100"/>
+      <c r="D39" s="99"/>
+      <c r="E39" s="99"/>
+      <c r="F39" s="101"/>
+      <c r="G39" s="99"/>
+      <c r="H39" s="102"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="103"/>
+      <c r="L39" s="104"/>
+      <c r="M39" s="105"/>
+      <c r="N39" s="105"/>
+      <c r="O39" s="105"/>
+      <c r="P39" s="105"/>
+      <c r="Q39" s="99"/>
+      <c r="R39" s="98"/>
+      <c r="S39" s="99"/>
+      <c r="T39" s="98"/>
       <c r="U39" s="13"/>
       <c r="V39" s="8"/>
       <c r="W39" s="8"/>
@@ -4282,24 +4279,24 @@
     </row>
     <row r="40" spans="1:31">
       <c r="A40" s="33"/>
-      <c r="B40" s="107"/>
-      <c r="C40" s="108"/>
-      <c r="D40" s="109"/>
-      <c r="E40" s="110"/>
+      <c r="B40" s="106"/>
+      <c r="C40" s="107"/>
+      <c r="D40" s="108"/>
+      <c r="E40" s="109"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="111"/>
-      <c r="H40" s="112"/>
+      <c r="G40" s="110"/>
+      <c r="H40" s="111"/>
       <c r="I40" s="33"/>
       <c r="J40" s="33"/>
       <c r="K40" s="49"/>
       <c r="L40" s="14"/>
-      <c r="M40" s="111"/>
-      <c r="N40" s="111"/>
-      <c r="O40" s="111"/>
-      <c r="P40" s="111"/>
-      <c r="Q40" s="108"/>
+      <c r="M40" s="110"/>
+      <c r="N40" s="110"/>
+      <c r="O40" s="110"/>
+      <c r="P40" s="110"/>
+      <c r="Q40" s="107"/>
       <c r="R40" s="33"/>
-      <c r="S40" s="108"/>
+      <c r="S40" s="107"/>
       <c r="T40" s="33"/>
       <c r="U40" s="15"/>
       <c r="V40" s="13"/>
@@ -4308,26 +4305,26 @@
       <c r="Y40" s="10"/>
     </row>
     <row r="41" spans="1:31">
-      <c r="A41" s="113"/>
-      <c r="B41" s="113"/>
-      <c r="C41" s="114"/>
-      <c r="D41" s="115"/>
-      <c r="E41" s="115"/>
-      <c r="F41" s="116"/>
-      <c r="G41" s="115"/>
-      <c r="H41" s="117"/>
-      <c r="I41" s="113"/>
-      <c r="J41" s="113"/>
-      <c r="K41" s="118"/>
+      <c r="A41" s="112"/>
+      <c r="B41" s="112"/>
+      <c r="C41" s="113"/>
+      <c r="D41" s="114"/>
+      <c r="E41" s="114"/>
+      <c r="F41" s="115"/>
+      <c r="G41" s="114"/>
+      <c r="H41" s="116"/>
+      <c r="I41" s="112"/>
+      <c r="J41" s="112"/>
+      <c r="K41" s="117"/>
       <c r="L41" s="37"/>
-      <c r="M41" s="119"/>
-      <c r="N41" s="119"/>
-      <c r="O41" s="119"/>
-      <c r="P41" s="119"/>
-      <c r="Q41" s="115"/>
-      <c r="R41" s="113"/>
-      <c r="S41" s="115"/>
-      <c r="T41" s="113"/>
+      <c r="M41" s="118"/>
+      <c r="N41" s="118"/>
+      <c r="O41" s="118"/>
+      <c r="P41" s="118"/>
+      <c r="Q41" s="114"/>
+      <c r="R41" s="112"/>
+      <c r="S41" s="114"/>
+      <c r="T41" s="112"/>
       <c r="U41" s="10"/>
       <c r="V41" s="10"/>
       <c r="W41" s="10"/>
@@ -4335,8 +4332,8 @@
       <c r="Y41" s="10"/>
     </row>
     <row r="42" spans="1:31">
-      <c r="A42" s="98"/>
-      <c r="B42" s="98"/>
+      <c r="A42" s="97"/>
+      <c r="B42" s="97"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -4362,26 +4359,26 @@
       <c r="Y42" s="10"/>
     </row>
     <row r="43" spans="1:31">
-      <c r="A43" s="113"/>
-      <c r="B43" s="115"/>
-      <c r="C43" s="114"/>
-      <c r="D43" s="115"/>
-      <c r="E43" s="115"/>
-      <c r="F43" s="116"/>
-      <c r="G43" s="115"/>
-      <c r="H43" s="117"/>
-      <c r="I43" s="113"/>
-      <c r="J43" s="113"/>
-      <c r="K43" s="118"/>
+      <c r="A43" s="112"/>
+      <c r="B43" s="114"/>
+      <c r="C43" s="113"/>
+      <c r="D43" s="114"/>
+      <c r="E43" s="114"/>
+      <c r="F43" s="115"/>
+      <c r="G43" s="114"/>
+      <c r="H43" s="116"/>
+      <c r="I43" s="112"/>
+      <c r="J43" s="112"/>
+      <c r="K43" s="117"/>
       <c r="L43" s="37"/>
-      <c r="M43" s="119"/>
-      <c r="N43" s="119"/>
-      <c r="O43" s="119"/>
-      <c r="P43" s="119"/>
-      <c r="Q43" s="115"/>
-      <c r="R43" s="113"/>
-      <c r="S43" s="115"/>
-      <c r="T43" s="120"/>
+      <c r="M43" s="118"/>
+      <c r="N43" s="118"/>
+      <c r="O43" s="118"/>
+      <c r="P43" s="118"/>
+      <c r="Q43" s="114"/>
+      <c r="R43" s="112"/>
+      <c r="S43" s="114"/>
+      <c r="T43" s="119"/>
       <c r="U43" s="10"/>
       <c r="V43" s="10"/>
       <c r="W43" s="10"/>
@@ -4389,7 +4386,7 @@
       <c r="Y43" s="10"/>
     </row>
     <row r="44" spans="1:31">
-      <c r="A44" s="98"/>
+      <c r="A44" s="97"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -4411,155 +4408,155 @@
       <c r="T44" s="36"/>
     </row>
     <row r="45" spans="1:31">
-      <c r="A45" s="98"/>
+      <c r="A45" s="97"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="F45" s="121"/>
+      <c r="F45" s="120"/>
       <c r="G45" s="1"/>
       <c r="H45" s="62"/>
-      <c r="I45" s="98"/>
-      <c r="J45" s="98"/>
-      <c r="K45" s="122"/>
-      <c r="L45" s="123"/>
+      <c r="I45" s="97"/>
+      <c r="J45" s="97"/>
+      <c r="K45" s="121"/>
+      <c r="L45" s="122"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="2"/>
-      <c r="R45" s="98"/>
+      <c r="R45" s="97"/>
       <c r="S45" s="2"/>
-      <c r="T45" s="98"/>
+      <c r="T45" s="97"/>
     </row>
     <row r="46" spans="1:31">
-      <c r="A46" s="120"/>
-      <c r="B46" s="124"/>
-      <c r="C46" s="125"/>
-      <c r="D46" s="126"/>
-      <c r="E46" s="126"/>
+      <c r="A46" s="119"/>
+      <c r="B46" s="123"/>
+      <c r="C46" s="124"/>
+      <c r="D46" s="125"/>
+      <c r="E46" s="125"/>
       <c r="F46" s="12"/>
-      <c r="G46" s="126"/>
-      <c r="H46" s="127"/>
-      <c r="I46" s="120"/>
-      <c r="J46" s="120"/>
-      <c r="K46" s="128"/>
+      <c r="G46" s="125"/>
+      <c r="H46" s="126"/>
+      <c r="I46" s="119"/>
+      <c r="J46" s="119"/>
+      <c r="K46" s="127"/>
       <c r="L46" s="13"/>
-      <c r="M46" s="129"/>
-      <c r="N46" s="129"/>
-      <c r="O46" s="129"/>
-      <c r="P46" s="129"/>
-      <c r="Q46" s="126"/>
-      <c r="R46" s="120"/>
-      <c r="S46" s="126"/>
-      <c r="T46" s="120"/>
-      <c r="U46" s="130"/>
-      <c r="V46" s="131"/>
+      <c r="M46" s="128"/>
+      <c r="N46" s="128"/>
+      <c r="O46" s="128"/>
+      <c r="P46" s="128"/>
+      <c r="Q46" s="125"/>
+      <c r="R46" s="119"/>
+      <c r="S46" s="125"/>
+      <c r="T46" s="119"/>
+      <c r="U46" s="129"/>
+      <c r="V46" s="130"/>
     </row>
     <row r="47" spans="1:31">
-      <c r="A47" s="98"/>
-      <c r="B47" s="138"/>
+      <c r="A47" s="97"/>
+      <c r="B47" s="137"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="121"/>
+      <c r="F47" s="120"/>
       <c r="G47" s="1"/>
       <c r="H47" s="62"/>
-      <c r="I47" s="98"/>
-      <c r="J47" s="98"/>
-      <c r="K47" s="122"/>
-      <c r="L47" s="123"/>
+      <c r="I47" s="97"/>
+      <c r="J47" s="97"/>
+      <c r="K47" s="121"/>
+      <c r="L47" s="122"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="98"/>
+      <c r="R47" s="97"/>
       <c r="S47" s="2"/>
-      <c r="T47" s="98"/>
+      <c r="T47" s="97"/>
     </row>
     <row r="48" spans="1:31">
-      <c r="A48" s="107"/>
-      <c r="B48" s="108"/>
-      <c r="C48" s="108"/>
-      <c r="D48" s="108"/>
-      <c r="E48" s="108"/>
+      <c r="A48" s="106"/>
+      <c r="B48" s="107"/>
+      <c r="C48" s="107"/>
+      <c r="D48" s="107"/>
+      <c r="E48" s="107"/>
       <c r="F48" s="9"/>
-      <c r="G48" s="111"/>
-      <c r="H48" s="139"/>
+      <c r="G48" s="110"/>
+      <c r="H48" s="138"/>
       <c r="I48" s="33"/>
       <c r="J48" s="33"/>
       <c r="K48" s="49"/>
       <c r="L48" s="14"/>
-      <c r="M48" s="111"/>
-      <c r="N48" s="111"/>
-      <c r="O48" s="111"/>
-      <c r="P48" s="111"/>
-      <c r="Q48" s="108"/>
+      <c r="M48" s="110"/>
+      <c r="N48" s="110"/>
+      <c r="O48" s="110"/>
+      <c r="P48" s="110"/>
+      <c r="Q48" s="107"/>
       <c r="R48" s="33"/>
-      <c r="S48" s="108"/>
+      <c r="S48" s="107"/>
       <c r="T48" s="33"/>
-      <c r="U48" s="140"/>
-      <c r="V48" s="140"/>
-      <c r="W48" s="140"/>
-      <c r="X48" s="140"/>
-      <c r="Y48" s="140"/>
-      <c r="Z48" s="140"/>
-      <c r="AA48" s="140"/>
-      <c r="AB48" s="140"/>
-      <c r="AC48" s="140"/>
-      <c r="AD48" s="140"/>
-      <c r="AE48" s="141"/>
+      <c r="U48" s="139"/>
+      <c r="V48" s="139"/>
+      <c r="W48" s="139"/>
+      <c r="X48" s="139"/>
+      <c r="Y48" s="139"/>
+      <c r="Z48" s="139"/>
+      <c r="AA48" s="139"/>
+      <c r="AB48" s="139"/>
+      <c r="AC48" s="139"/>
+      <c r="AD48" s="139"/>
+      <c r="AE48" s="140"/>
     </row>
     <row r="49" spans="1:31">
-      <c r="A49" s="99"/>
-      <c r="B49" s="132"/>
-      <c r="C49" s="133"/>
-      <c r="D49" s="132"/>
-      <c r="E49" s="132"/>
-      <c r="F49" s="102"/>
-      <c r="G49" s="132"/>
-      <c r="H49" s="134"/>
-      <c r="I49" s="99"/>
-      <c r="J49" s="99"/>
-      <c r="K49" s="104"/>
-      <c r="L49" s="105"/>
-      <c r="M49" s="106"/>
-      <c r="N49" s="106"/>
-      <c r="O49" s="106"/>
-      <c r="P49" s="106"/>
-      <c r="Q49" s="132"/>
-      <c r="R49" s="99"/>
-      <c r="S49" s="132"/>
-      <c r="T49" s="99"/>
-      <c r="AE49" s="142"/>
+      <c r="A49" s="98"/>
+      <c r="B49" s="131"/>
+      <c r="C49" s="132"/>
+      <c r="D49" s="131"/>
+      <c r="E49" s="131"/>
+      <c r="F49" s="101"/>
+      <c r="G49" s="131"/>
+      <c r="H49" s="133"/>
+      <c r="I49" s="98"/>
+      <c r="J49" s="98"/>
+      <c r="K49" s="103"/>
+      <c r="L49" s="104"/>
+      <c r="M49" s="105"/>
+      <c r="N49" s="105"/>
+      <c r="O49" s="105"/>
+      <c r="P49" s="105"/>
+      <c r="Q49" s="131"/>
+      <c r="R49" s="98"/>
+      <c r="S49" s="131"/>
+      <c r="T49" s="98"/>
+      <c r="AE49" s="141"/>
     </row>
     <row r="50" spans="1:31">
       <c r="A50" s="33"/>
-      <c r="B50" s="135"/>
-      <c r="C50" s="135"/>
-      <c r="D50" s="135"/>
-      <c r="E50" s="135"/>
+      <c r="B50" s="134"/>
+      <c r="C50" s="134"/>
+      <c r="D50" s="134"/>
+      <c r="E50" s="134"/>
       <c r="F50" s="9"/>
-      <c r="G50" s="136"/>
-      <c r="H50" s="137"/>
+      <c r="G50" s="135"/>
+      <c r="H50" s="136"/>
       <c r="I50" s="33"/>
       <c r="J50" s="33"/>
       <c r="K50" s="49"/>
       <c r="L50" s="14"/>
-      <c r="M50" s="136"/>
-      <c r="N50" s="136"/>
-      <c r="O50" s="136"/>
-      <c r="P50" s="136"/>
-      <c r="Q50" s="135"/>
+      <c r="M50" s="135"/>
+      <c r="N50" s="135"/>
+      <c r="O50" s="135"/>
+      <c r="P50" s="135"/>
+      <c r="Q50" s="134"/>
       <c r="R50" s="33"/>
-      <c r="S50" s="135"/>
+      <c r="S50" s="134"/>
       <c r="T50" s="33"/>
-      <c r="U50" s="131"/>
-      <c r="AE50" s="142"/>
+      <c r="U50" s="130"/>
+      <c r="AE50" s="141"/>
     </row>
     <row r="51" spans="1:31">
-      <c r="A51" s="98"/>
+      <c r="A51" s="97"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -4579,40 +4576,40 @@
       <c r="R51" s="36"/>
       <c r="S51" s="2"/>
       <c r="T51" s="36"/>
-      <c r="AE51" s="142"/>
+      <c r="AE51" s="141"/>
     </row>
     <row r="52" spans="1:31">
-      <c r="A52" s="113"/>
-      <c r="B52" s="115"/>
-      <c r="C52" s="114"/>
-      <c r="D52" s="115"/>
-      <c r="E52" s="115"/>
-      <c r="F52" s="116"/>
-      <c r="G52" s="115"/>
-      <c r="H52" s="117"/>
-      <c r="I52" s="113"/>
-      <c r="J52" s="113"/>
-      <c r="K52" s="118"/>
+      <c r="A52" s="112"/>
+      <c r="B52" s="114"/>
+      <c r="C52" s="113"/>
+      <c r="D52" s="114"/>
+      <c r="E52" s="114"/>
+      <c r="F52" s="115"/>
+      <c r="G52" s="114"/>
+      <c r="H52" s="116"/>
+      <c r="I52" s="112"/>
+      <c r="J52" s="112"/>
+      <c r="K52" s="117"/>
       <c r="L52" s="37"/>
-      <c r="M52" s="119"/>
-      <c r="N52" s="119"/>
-      <c r="O52" s="119"/>
-      <c r="P52" s="119"/>
-      <c r="Q52" s="115"/>
-      <c r="R52" s="113"/>
-      <c r="S52" s="115"/>
-      <c r="T52" s="113"/>
-      <c r="U52" s="143"/>
-      <c r="V52" s="143"/>
-      <c r="W52" s="143"/>
-      <c r="X52" s="143"/>
-      <c r="Y52" s="143"/>
-      <c r="Z52" s="143"/>
-      <c r="AA52" s="143"/>
-      <c r="AB52" s="143"/>
-      <c r="AC52" s="143"/>
-      <c r="AD52" s="143"/>
-      <c r="AE52" s="144"/>
+      <c r="M52" s="118"/>
+      <c r="N52" s="118"/>
+      <c r="O52" s="118"/>
+      <c r="P52" s="118"/>
+      <c r="Q52" s="114"/>
+      <c r="R52" s="112"/>
+      <c r="S52" s="114"/>
+      <c r="T52" s="112"/>
+      <c r="U52" s="142"/>
+      <c r="V52" s="142"/>
+      <c r="W52" s="142"/>
+      <c r="X52" s="142"/>
+      <c r="Y52" s="142"/>
+      <c r="Z52" s="142"/>
+      <c r="AA52" s="142"/>
+      <c r="AB52" s="142"/>
+      <c r="AC52" s="142"/>
+      <c r="AD52" s="142"/>
+      <c r="AE52" s="143"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4624,8 +4621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{965FBAF6-7E35-482C-9958-4C835D5BDDCC}">
   <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="V32" activeCellId="8" sqref="V4 V6 V10 V13 V18 V22 V25 V29 V32"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4654,19 +4651,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="81" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E1" s="81" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>9</v>
@@ -4675,16 +4672,16 @@
         <v>15</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>7</v>
@@ -4693,10 +4690,10 @@
         <v>8</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>13</v>
@@ -4708,18 +4705,18 @@
         <v>12</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="80">
         <v>46</v>
@@ -4760,16 +4757,16 @@
         <v>0.13800886937000487</v>
       </c>
       <c r="M2" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N2" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O2" s="1">
-        <v>0.87</v>
+        <v>0.86599999999999999</v>
       </c>
       <c r="P2" s="1">
-        <v>0.14699999999999999</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="Q2" s="7">
         <v>119</v>
@@ -4785,10 +4782,10 @@
         <f t="shared" ref="T2:T32" si="3">S2/(G2/60)</f>
         <v>1.1500739114167071</v>
       </c>
-      <c r="U2" s="145">
+      <c r="U2" s="144">
         <v>10</v>
       </c>
-      <c r="V2" s="145">
+      <c r="V2" s="144">
         <f>U2/(G2/60)</f>
         <v>0.46002956456668287</v>
       </c>
@@ -4798,7 +4795,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" s="80">
         <v>46</v>
@@ -4839,10 +4836,10 @@
         <v>0.16739530121389493</v>
       </c>
       <c r="M3" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N3" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O3" s="1">
         <v>0.93200000000000005</v>
@@ -4864,10 +4861,10 @@
         <f t="shared" si="3"/>
         <v>1.3391624097111594</v>
       </c>
-      <c r="U3" s="145">
+      <c r="U3" s="144">
         <v>4</v>
       </c>
-      <c r="V3" s="145">
+      <c r="V3" s="144">
         <f t="shared" ref="V3:V32" si="7">U3/(G3/60)</f>
         <v>0.6695812048555797</v>
       </c>
@@ -4877,13 +4874,13 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="53" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="23">
         <v>46</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="3">
         <f>SUM(D2:D3)</f>
@@ -4922,16 +4919,16 @@
         <v>0.14434379805821507</v>
       </c>
       <c r="M4" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N4" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O4" s="41">
-        <v>0.88300000000000001</v>
+        <v>0.88</v>
       </c>
       <c r="P4" s="41">
-        <v>0.13900000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="Q4" s="3">
         <f xml:space="preserve"> SUM(Q2:Q3)</f>
@@ -4949,11 +4946,11 @@
         <f t="shared" si="3"/>
         <v>1.1908363339802743</v>
       </c>
-      <c r="U4" s="146">
+      <c r="U4" s="145">
         <f>SUM(U2:U3)</f>
         <v>14</v>
       </c>
-      <c r="V4" s="147">
+      <c r="V4" s="146">
         <f t="shared" si="7"/>
         <v>0.50520329320375279</v>
       </c>
@@ -4963,7 +4960,7 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" s="92">
         <v>47</v>
@@ -5004,16 +5001,16 @@
         <v>0.18847555733792934</v>
       </c>
       <c r="M5" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N5" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O5" s="1">
-        <v>0.80300000000000005</v>
+        <v>0.80100000000000005</v>
       </c>
       <c r="P5" s="1">
-        <v>0.184</v>
+        <v>0.185</v>
       </c>
       <c r="Q5" s="2">
         <v>119</v>
@@ -5029,10 +5026,10 @@
         <f t="shared" si="3"/>
         <v>1.5706296444827446</v>
       </c>
-      <c r="U5" s="145">
+      <c r="U5" s="144">
         <v>12</v>
       </c>
-      <c r="V5" s="145">
+      <c r="V5" s="144">
         <f t="shared" si="7"/>
         <v>0.75390222935171747</v>
       </c>
@@ -5042,13 +5039,13 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="53" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="90">
         <v>47</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3">
         <f>SUM(D5)</f>
@@ -5087,16 +5084,16 @@
         <v>0.18847555733792934</v>
       </c>
       <c r="M6" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N6" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O6" s="41">
-        <v>0.80300000000000005</v>
+        <v>0.80100000000000005</v>
       </c>
       <c r="P6" s="41">
-        <v>0.184</v>
+        <v>0.185</v>
       </c>
       <c r="Q6" s="3">
         <f>SUM(Q5)</f>
@@ -5114,11 +5111,11 @@
         <f t="shared" si="3"/>
         <v>1.5706296444827446</v>
       </c>
-      <c r="U6" s="146">
+      <c r="U6" s="145">
         <f>SUM(U5)</f>
         <v>12</v>
       </c>
-      <c r="V6" s="147">
+      <c r="V6" s="146">
         <f t="shared" si="7"/>
         <v>0.75390222935171747</v>
       </c>
@@ -5128,7 +5125,7 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="91" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="91">
         <v>49</v>
@@ -5169,10 +5166,10 @@
         <v>8.9789040648995191E-2</v>
       </c>
       <c r="M7" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N7" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O7" s="1">
         <v>0.89600000000000002</v>
@@ -5194,10 +5191,10 @@
         <f t="shared" si="3"/>
         <v>2.2447260162248801</v>
       </c>
-      <c r="U7" s="145">
+      <c r="U7" s="144">
         <v>3</v>
       </c>
-      <c r="V7" s="145">
+      <c r="V7" s="144">
         <f t="shared" si="7"/>
         <v>0.26936712194698559</v>
       </c>
@@ -5207,7 +5204,7 @@
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="14">
         <v>49</v>
@@ -5248,10 +5245,10 @@
         <v>0</v>
       </c>
       <c r="M8" s="51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N8" s="51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O8" s="1">
         <v>0.89400000000000002</v>
@@ -5273,10 +5270,10 @@
         <f t="shared" si="3"/>
         <v>2.4614495968966041</v>
       </c>
-      <c r="U8" s="145">
-        <v>0</v>
-      </c>
-      <c r="V8" s="145">
+      <c r="U8" s="144">
+        <v>0</v>
+      </c>
+      <c r="V8" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5286,7 +5283,7 @@
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" s="14">
         <v>49</v>
@@ -5327,10 +5324,10 @@
         <v>8.7446857815781529E-2</v>
       </c>
       <c r="M9" s="51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N9" s="51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O9" s="1">
         <v>0.90600000000000003</v>
@@ -5352,10 +5349,10 @@
         <f t="shared" si="3"/>
         <v>1.9238308719471937</v>
       </c>
-      <c r="U9" s="145">
+      <c r="U9" s="144">
         <v>1</v>
       </c>
-      <c r="V9" s="145">
+      <c r="V9" s="144">
         <f t="shared" si="7"/>
         <v>8.7446857815781529E-2</v>
       </c>
@@ -5365,13 +5362,13 @@
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="53" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="23">
         <v>49</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="3">
         <f>SUM(D7:D9)</f>
@@ -5410,10 +5407,10 @@
         <v>6.1107232499270539E-2</v>
       </c>
       <c r="M10" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N10" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O10" s="41">
         <v>0.89900000000000002</v>
@@ -5437,11 +5434,11 @@
         <f t="shared" si="3"/>
         <v>2.1998603699737393</v>
       </c>
-      <c r="U10" s="146">
+      <c r="U10" s="145">
         <f>SUM(U7:U9)</f>
         <v>4</v>
       </c>
-      <c r="V10" s="147">
+      <c r="V10" s="146">
         <f t="shared" si="7"/>
         <v>0.12221446499854108</v>
       </c>
@@ -5451,7 +5448,7 @@
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" s="83">
         <v>53</v>
@@ -5492,10 +5489,10 @@
         <v>0.53642313056538993</v>
       </c>
       <c r="M11" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N11" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O11" s="1">
         <v>0.80900000000000005</v>
@@ -5517,10 +5514,10 @@
         <f t="shared" si="3"/>
         <v>2.0690606464665042</v>
       </c>
-      <c r="U11" s="145">
+      <c r="U11" s="144">
         <v>6</v>
       </c>
-      <c r="V11" s="145">
+      <c r="V11" s="144">
         <f t="shared" si="7"/>
         <v>0.45979125477033428</v>
       </c>
@@ -5530,7 +5527,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="80">
         <v>53</v>
@@ -5571,10 +5568,10 @@
         <v>0.33367395883297535</v>
       </c>
       <c r="M12" s="51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N12" s="51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O12" s="1">
         <v>0.83899999999999997</v>
@@ -5596,10 +5593,10 @@
         <f t="shared" si="3"/>
         <v>1.9186252632896081</v>
       </c>
-      <c r="U12" s="145">
+      <c r="U12" s="144">
         <v>1</v>
       </c>
-      <c r="V12" s="145">
+      <c r="V12" s="144">
         <f t="shared" si="7"/>
         <v>8.3418489708243837E-2</v>
       </c>
@@ -5609,13 +5606,13 @@
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="53" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="53">
         <v>53</v>
       </c>
       <c r="C13" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" s="84">
         <f>SUM(D11:D12)</f>
@@ -5654,10 +5651,10 @@
         <v>0.43934713016457544</v>
       </c>
       <c r="M13" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N13" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O13" s="58">
         <v>0.82299999999999995</v>
@@ -5681,11 +5678,11 @@
         <f t="shared" si="3"/>
         <v>1.9970324098389793</v>
       </c>
-      <c r="U13" s="146">
+      <c r="U13" s="145">
         <f>SUM(U11:U12)</f>
         <v>7</v>
       </c>
-      <c r="V13" s="147">
+      <c r="V13" s="146">
         <f t="shared" si="7"/>
         <v>0.27958453737745709</v>
       </c>
@@ -5695,7 +5692,7 @@
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="48" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="48">
         <v>55</v>
@@ -5736,10 +5733,10 @@
         <v>0</v>
       </c>
       <c r="M14" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N14" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O14" s="50">
         <v>0.94299999999999995</v>
@@ -5761,10 +5758,10 @@
         <f t="shared" si="3"/>
         <v>1.8322702625191858</v>
       </c>
-      <c r="U14" s="145">
+      <c r="U14" s="144">
         <v>5</v>
       </c>
-      <c r="V14" s="145">
+      <c r="V14" s="144">
         <f t="shared" si="7"/>
         <v>0.39831962228677953</v>
       </c>
@@ -5774,7 +5771,7 @@
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="48" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" s="48">
         <v>55</v>
@@ -5815,10 +5812,10 @@
         <v>0</v>
       </c>
       <c r="M15" s="51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N15" s="51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O15" s="50">
         <v>0.93200000000000005</v>
@@ -5840,10 +5837,10 @@
         <f t="shared" si="3"/>
         <v>1.7226438929663928</v>
       </c>
-      <c r="U15" s="145">
-        <v>0</v>
-      </c>
-      <c r="V15" s="145">
+      <c r="U15" s="144">
+        <v>0</v>
+      </c>
+      <c r="V15" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5853,7 +5850,7 @@
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="48" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="48">
         <v>55</v>
@@ -5894,16 +5891,16 @@
         <v>0</v>
       </c>
       <c r="M16" s="74" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N16" s="51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O16" s="9">
-        <v>0.96</v>
+        <v>0.95899999999999996</v>
       </c>
       <c r="P16" s="9">
-        <v>0.09</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="Q16" s="9">
         <v>112</v>
@@ -5919,10 +5916,10 @@
         <f t="shared" si="3"/>
         <v>1.9134206162374032</v>
       </c>
-      <c r="U16" s="145">
-        <v>0</v>
-      </c>
-      <c r="V16" s="145">
+      <c r="U16" s="144">
+        <v>0</v>
+      </c>
+      <c r="V16" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5932,7 +5929,7 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="48" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" s="48">
         <v>55</v>
@@ -5973,16 +5970,16 @@
         <v>8.6376795737593062E-2</v>
       </c>
       <c r="M17" s="76" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N17" s="73" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O17" s="50">
-        <v>1.002</v>
+        <v>0.998</v>
       </c>
       <c r="P17" s="50">
-        <v>9.4E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="Q17" s="9">
         <v>108</v>
@@ -5998,10 +5995,10 @@
         <f t="shared" si="3"/>
         <v>2.0730430977022336</v>
       </c>
-      <c r="U17" s="145">
+      <c r="U17" s="144">
         <v>2</v>
       </c>
-      <c r="V17" s="145">
+      <c r="V17" s="144">
         <f t="shared" si="7"/>
         <v>0.17275359147518612</v>
       </c>
@@ -6011,13 +6008,13 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="53" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="53">
         <v>55</v>
       </c>
       <c r="C18" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D18" s="56">
         <f>SUM(D14:D17)</f>
@@ -6056,16 +6053,16 @@
         <v>2.0661704873028659E-2</v>
       </c>
       <c r="M18" s="75" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N18" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O18" s="58">
-        <v>0.95899999999999996</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="P18" s="58">
-        <v>9.8000000000000004E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="Q18" s="56">
         <f>SUM(Q14:Q17)</f>
@@ -6083,11 +6080,11 @@
         <f t="shared" si="3"/>
         <v>1.880215143445608</v>
       </c>
-      <c r="U18" s="146">
+      <c r="U18" s="145">
         <f>SUM(U14:U17)</f>
         <v>7</v>
       </c>
-      <c r="V18" s="147">
+      <c r="V18" s="146">
         <f t="shared" si="7"/>
         <v>0.14463193411120062</v>
       </c>
@@ -6097,7 +6094,7 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" s="36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" s="36">
         <v>56</v>
@@ -6138,10 +6135,10 @@
         <v>0</v>
       </c>
       <c r="M19" s="55" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N19" s="55" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O19" s="31">
         <v>0.876</v>
@@ -6163,10 +6160,10 @@
         <f t="shared" si="3"/>
         <v>1.8637793393307409</v>
       </c>
-      <c r="U19" s="145">
-        <v>0</v>
-      </c>
-      <c r="V19" s="145">
+      <c r="U19" s="144">
+        <v>0</v>
+      </c>
+      <c r="V19" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -6176,7 +6173,7 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="33">
         <v>56</v>
@@ -6217,10 +6214,10 @@
         <v>0</v>
       </c>
       <c r="M20" s="44" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N20" s="44" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O20" s="1">
         <v>0.90600000000000003</v>
@@ -6242,10 +6239,10 @@
         <f t="shared" si="3"/>
         <v>1.9764374285689734</v>
       </c>
-      <c r="U20" s="145">
+      <c r="U20" s="144">
         <v>1</v>
       </c>
-      <c r="V20" s="145">
+      <c r="V20" s="144">
         <f t="shared" si="7"/>
         <v>8.593206211169449E-2</v>
       </c>
@@ -6255,7 +6252,7 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" s="33">
         <v>56</v>
@@ -6296,10 +6293,10 @@
         <v>9.0379821198587063E-2</v>
       </c>
       <c r="M21" s="44" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N21" s="44" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O21" s="1">
         <v>0.91700000000000004</v>
@@ -6321,10 +6318,10 @@
         <f t="shared" si="3"/>
         <v>1.7172166027731541</v>
       </c>
-      <c r="U21" s="145">
-        <v>0</v>
-      </c>
-      <c r="V21" s="145">
+      <c r="U21" s="144">
+        <v>0</v>
+      </c>
+      <c r="V21" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -6334,13 +6331,13 @@
     </row>
     <row r="22" spans="1:25">
       <c r="A22" s="34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" s="40">
         <v>56</v>
       </c>
       <c r="C22" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D22" s="35">
         <f>SUM(D19:D21)</f>
@@ -6379,10 +6376,10 @@
         <v>2.8537156805017977E-2</v>
       </c>
       <c r="M22" s="77" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N22" s="78" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O22" s="41">
         <v>0.89900000000000002</v>
@@ -6406,11 +6403,11 @@
         <f t="shared" si="3"/>
         <v>1.8549151923261684</v>
       </c>
-      <c r="U22" s="146">
+      <c r="U22" s="145">
         <f>SUM(U19:U21)</f>
         <v>1</v>
       </c>
-      <c r="V22" s="147">
+      <c r="V22" s="146">
         <f t="shared" si="7"/>
         <v>2.8537156805017977E-2</v>
       </c>
@@ -6461,7 +6458,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="31">
-        <v>0.73899999999999999</v>
+        <v>0.74099999999999999</v>
       </c>
       <c r="N23" s="31">
         <v>6.7000000000000004E-2</v>
@@ -6488,10 +6485,10 @@
         <f t="shared" si="3"/>
         <v>2.0436754169542128</v>
       </c>
-      <c r="U23" s="145">
+      <c r="U23" s="144">
         <v>1</v>
       </c>
-      <c r="V23" s="145">
+      <c r="V23" s="144">
         <f t="shared" si="7"/>
         <v>8.8855452911052735E-2</v>
       </c>
@@ -6542,10 +6539,10 @@
         <v>0</v>
       </c>
       <c r="M24" s="1">
-        <v>0.75800000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="N24" s="1">
-        <v>6.6000000000000003E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="O24" s="1">
         <v>0.96499999999999997</v>
@@ -6567,10 +6564,10 @@
         <f t="shared" si="3"/>
         <v>2.2853963175309775</v>
       </c>
-      <c r="U24" s="145">
-        <v>0</v>
-      </c>
-      <c r="V24" s="145">
+      <c r="U24" s="144">
+        <v>0</v>
+      </c>
+      <c r="V24" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -6580,13 +6577,13 @@
     </row>
     <row r="25" spans="1:25">
       <c r="A25" s="34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" s="34">
         <v>67</v>
       </c>
       <c r="C25" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D25" s="34">
         <f>SUM(D23:D24)</f>
@@ -6625,10 +6622,10 @@
         <v>0</v>
       </c>
       <c r="M25" s="79">
-        <v>0.748</v>
+        <v>0.75</v>
       </c>
       <c r="N25" s="41">
-        <v>6.7000000000000004E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="O25" s="41">
         <v>0.96699999999999997</v>
@@ -6652,11 +6649,11 @@
         <f t="shared" si="3"/>
         <v>2.157787423539272</v>
       </c>
-      <c r="U25" s="146">
+      <c r="U25" s="145">
         <f>SUM(U23:U24)</f>
         <v>1</v>
       </c>
-      <c r="V25" s="147">
+      <c r="V25" s="146">
         <f t="shared" si="7"/>
         <v>4.6908422250853739E-2</v>
       </c>
@@ -6707,7 +6704,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="1">
-        <v>0.69599999999999995</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="N26" s="1">
         <v>0.10100000000000001</v>
@@ -6732,10 +6729,10 @@
         <f t="shared" si="3"/>
         <v>1.7066360837480459</v>
       </c>
-      <c r="U26" s="145">
+      <c r="U26" s="144">
         <v>2</v>
       </c>
-      <c r="V26" s="145">
+      <c r="V26" s="144">
         <f t="shared" si="7"/>
         <v>0.13653088669984367</v>
       </c>
@@ -6786,7 +6783,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="1">
-        <v>0.72499999999999998</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="N27" s="1">
         <v>8.1000000000000003E-2</v>
@@ -6811,10 +6808,10 @@
         <f t="shared" si="3"/>
         <v>2.0790874602791622</v>
       </c>
-      <c r="U27" s="145">
-        <v>0</v>
-      </c>
-      <c r="V27" s="145">
+      <c r="U27" s="144">
+        <v>0</v>
+      </c>
+      <c r="V27" s="144">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -6865,7 +6862,7 @@
         <v>6.750857358884578E-2</v>
       </c>
       <c r="M28" s="1">
-        <v>0.76900000000000002</v>
+        <v>0.77100000000000002</v>
       </c>
       <c r="N28" s="1">
         <v>7.0999999999999994E-2</v>
@@ -6890,10 +6887,10 @@
         <f t="shared" si="3"/>
         <v>1.4851886189546073</v>
       </c>
-      <c r="U28" s="145">
+      <c r="U28" s="144">
         <v>6</v>
       </c>
-      <c r="V28" s="145">
+      <c r="V28" s="144">
         <f t="shared" si="7"/>
         <v>0.40505144153307476</v>
       </c>
@@ -6903,13 +6900,13 @@
     </row>
     <row r="29" spans="1:25">
       <c r="A29" s="34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" s="40">
         <v>68</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D29" s="35">
         <f>SUM(D26:D28)</f>
@@ -6948,7 +6945,7 @@
         <v>2.3558180460373963E-2</v>
       </c>
       <c r="M29" s="41">
-        <v>0.72899999999999998</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="N29" s="41">
         <v>9.0999999999999998E-2</v>
@@ -6975,11 +6972,11 @@
         <f t="shared" si="3"/>
         <v>1.7433053540676733</v>
       </c>
-      <c r="U29" s="146">
+      <c r="U29" s="145">
         <f>SUM(U26:U28)</f>
         <v>8</v>
       </c>
-      <c r="V29" s="147">
+      <c r="V29" s="146">
         <f t="shared" si="7"/>
         <v>0.18846544368299173</v>
       </c>
@@ -7030,7 +7027,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="1">
-        <v>0.76</v>
+        <v>0.76100000000000001</v>
       </c>
       <c r="N30" s="1">
         <v>6.5000000000000002E-2</v>
@@ -7055,10 +7052,10 @@
         <f t="shared" si="3"/>
         <v>1.8175891739541896</v>
       </c>
-      <c r="U30" s="145">
+      <c r="U30" s="144">
         <v>7</v>
       </c>
-      <c r="V30" s="145">
+      <c r="V30" s="144">
         <f t="shared" si="7"/>
         <v>0.50892496870717308</v>
       </c>
@@ -7109,7 +7106,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="30">
-        <v>0.77700000000000002</v>
+        <v>0.78</v>
       </c>
       <c r="N31" s="30">
         <v>7.0999999999999994E-2</v>
@@ -7134,10 +7131,10 @@
         <f t="shared" si="3"/>
         <v>1.3564770236427779</v>
       </c>
-      <c r="U31" s="145">
+      <c r="U31" s="144">
         <v>11</v>
       </c>
-      <c r="V31" s="145">
+      <c r="V31" s="144">
         <f t="shared" si="7"/>
         <v>0.67823851182138895</v>
       </c>
@@ -7147,13 +7144,13 @@
     </row>
     <row r="32" spans="1:25">
       <c r="A32" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B32" s="19">
         <v>81</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D32" s="19">
         <f>SUM(D30:D31)</f>
@@ -7192,13 +7189,13 @@
         <v>0</v>
       </c>
       <c r="M32" s="39">
-        <v>0.76900000000000002</v>
+        <v>0.77100000000000002</v>
       </c>
       <c r="N32" s="39">
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="O32" s="39">
-        <v>0.97599999999999998</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="P32" s="39">
         <v>8.5999999999999993E-2</v>
@@ -7219,11 +7216,11 @@
         <f t="shared" si="3"/>
         <v>1.5680796806900439</v>
       </c>
-      <c r="U32" s="146">
+      <c r="U32" s="145">
         <f>SUM(U30:U31)</f>
         <v>18</v>
       </c>
-      <c r="V32" s="147">
+      <c r="V32" s="146">
         <f t="shared" si="7"/>
         <v>0.60054115430682531</v>
       </c>

</xml_diff>